<commit_message>
Minor bug fix + feature add
Fixed bug that wouldn't compile to walk inbetween rooms.
Added ability to lock rooms and prevent player from entering them.
</commit_message>
<xml_diff>
--- a/rooms.xlsx
+++ b/rooms.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\C4GD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="107" documentId="C832CFACED3E90FD9C08E0A943A5C402EA6626A5" xr6:coauthVersionLast="11" xr6:coauthVersionMax="11" xr10:uidLastSave="{128930B8-EF5B-4D00-B390-882DC46CDA93}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,15 +25,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="34">
   <si>
     <t>rooms[5][5]</t>
+  </si>
+  <si>
+    <t>Key:</t>
+  </si>
+  <si>
+    <t>Q = Quest</t>
+  </si>
+  <si>
+    <t>D = DROP</t>
+  </si>
+  <si>
+    <t>E = Enemy</t>
+  </si>
+  <si>
+    <t>E: EZ</t>
+  </si>
+  <si>
+    <t>NPC:</t>
+  </si>
+  <si>
+    <t>Items:</t>
+  </si>
+  <si>
+    <t>Room1</t>
+  </si>
+  <si>
+    <t>Room2</t>
+  </si>
+  <si>
+    <t>Room5</t>
+  </si>
+  <si>
+    <t>Room3</t>
+  </si>
+  <si>
+    <t>Room4</t>
+  </si>
+  <si>
+    <t>WORLD</t>
+  </si>
+  <si>
+    <t>LOCK UNTIL Q2</t>
+  </si>
+  <si>
+    <t>Q1: Get QI1</t>
+  </si>
+  <si>
+    <t>I = Item</t>
+  </si>
+  <si>
+    <t>F = Friendly</t>
+  </si>
+  <si>
+    <t>F: Bel Drock</t>
+  </si>
+  <si>
+    <t>F: Charlie</t>
+  </si>
+  <si>
+    <t>G:Sword</t>
+  </si>
+  <si>
+    <t>G = GIVE</t>
+  </si>
+  <si>
+    <t>Q3: Get XP</t>
+  </si>
+  <si>
+    <t>LOCK:</t>
+  </si>
+  <si>
+    <t>DQI1: Shield</t>
+  </si>
+  <si>
+    <t>D: QI2 Some Item</t>
+  </si>
+  <si>
+    <t>E: Respawn (Diplodicus)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -42,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -61,8 +140,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -85,11 +170,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF505050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF505050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF505050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF505050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF505050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF505050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF505050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF505050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF505050"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF505050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF505050"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -103,6 +273,27 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -129,15 +320,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>329890</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>9292</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>197470</xdr:colOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>497205</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>123592</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -145,6 +336,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -165,23 +359,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -454,20 +635,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
@@ -487,7 +673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C3" s="5">
         <v>1</v>
       </c>
@@ -507,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C4" s="5">
         <v>2</v>
       </c>
@@ -528,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C5" s="5">
         <v>3</v>
       </c>
@@ -550,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C6" s="5">
         <v>4</v>
       </c>
@@ -573,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -597,45 +783,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -645,56 +811,155 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="13"/>
+      <c r="I17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H19" s="12"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L23" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L22:M22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -711,8 +976,8 @@
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>200025</xdr:colOff>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>497205</xdr:colOff>
                 <xdr:row>12</xdr:row>
                 <xdr:rowOff>123825</xdr:rowOff>
               </to>

</xml_diff>